<commit_message>
Refactoring + javadoc SaveProject
</commit_message>
<xml_diff>
--- a/Dossiers personnels/Jérémie/Journal_Travail_Jeremie.xlsx
+++ b/Dossiers personnels/Jérémie/Journal_Travail_Jeremie.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10513"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490CFBF7-AE5C-41B4-A950-12FFDC208748}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D13503E-1D20-B74B-A08D-D3AF91C72817}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -201,7 +201,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -228,18 +228,59 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -249,7 +290,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -258,20 +298,30 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -556,31 +606,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:3" s="5" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="10"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-    </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="13"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
+    </row>
+    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -591,440 +641,440 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>43150</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="8">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C5" s="7">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>43152</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>43153</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>43157</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="8">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="C8" s="7">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>43158</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>43161</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="8">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C10" s="7">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>5</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="8">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C11" s="7">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>43106</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>43166</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>43168</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>43170</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>43171</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="8">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C17" s="7">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>43172</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>43204</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>43174</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>43174</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>43175</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="8">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C22" s="7">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>43178</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>43179</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>43183</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>43185</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="8">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C26" s="7">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>43186</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="7">
         <v>3.5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>43199</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="8">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C28" s="7">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>43205</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="7">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>43206</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="8">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="7">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>43211</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="12">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="10">
         <v>43213</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="11">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="C32" s="9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>43218</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="7">
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>43220</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="11">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C34" s="9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>43225</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C35" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>43441</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C36" s="11">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C36" s="9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>43443</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C37" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>43230</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38" s="7">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>43231</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C39" s="7">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="14">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="12">
         <v>43235</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="8">
+      <c r="C40" s="15">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="14">
         <v>43236</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C41" s="15">
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="14">
         <v>43237</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C42" s="15">
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="3">
-        <v>43237</v>
-      </c>
-      <c r="B43" s="15" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="14">
+        <v>43238</v>
+      </c>
+      <c r="B43" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="8">
+      <c r="C43" s="15">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="5" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B44" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="9">
+      <c r="C44" s="8">
         <f>SUM(C14:C43)</f>
         <v>95.5</v>
       </c>

</xml_diff>